<commit_message>
Allow use of multi parameter in jxls template
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls1.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls1.xlsx
@@ -56,7 +56,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="jdbc.query('select o.order_id, c.name city_name, i.name item_name, o.order_date, o.volume from orders o, cities c, items i where o.city_id=c.city_id and o.item_id=i.item_id and order_date&gt;=? and o.city_id=? order by o.order_date', order_date.value, cityId.value)" var="item" lastCell="E10")</t>
+jx:each(items="jdbc.query('select o.order_id, c.name city_name, i.name item_name, o.order_date, o.volume from orders o, cities c, items i where o.city_id=c.city_id and o.item_id=i.item_id and order_date&gt;=? and o.city_id=? and o.item_id in(' + item.sqlValue + ') order by o.order_date', order_date.value, cityId.value)" var="item" lastCell="E10")</t>
         </r>
       </text>
     </comment>
@@ -520,7 +520,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected using of all values for multi-value parameters when nothing is selected Allow use of localized parameter labels in jxls templates
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls1.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls1.xlsx
@@ -115,10 +115,10 @@
     <t>${cityId.parameter.label}</t>
   </si>
   <si>
-    <t>${item.nameAndDisplayValues}</t>
-  </si>
-  <si>
     <t>${cityId.value}</t>
+  </si>
+  <si>
+    <t>${item.getLocalizedLabelAndDisplayValues(locale)}</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,12 +549,12 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>